<commit_message>
Added test script, accuracy computation, figure plotting. Added images and some workspace backup
</commit_message>
<xml_diff>
--- a/Assignment 3 - kNN classifier/tables.xlsx
+++ b/Assignment 3 - kNN classifier/tables.xlsx
@@ -24,12 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>k</t>
   </si>
   <si>
     <t>error</t>
+  </si>
+  <si>
+    <t>error rate</t>
   </si>
 </sst>
 </file>
@@ -356,10 +359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N28"/>
+  <dimension ref="A2:N210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,6 +450,14 @@
       </c>
       <c r="N3" s="1"/>
     </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3.6999999999999998E-2</v>
@@ -454,6 +465,12 @@
       <c r="B10">
         <v>21</v>
       </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>3.09E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -462,6 +479,12 @@
       <c r="B11">
         <v>31</v>
       </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>3.56E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -470,6 +493,12 @@
       <c r="B12">
         <v>41</v>
       </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>2.92E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -478,6 +507,12 @@
       <c r="B13">
         <v>51</v>
       </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>3.1600000000000003E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -486,6 +521,12 @@
       <c r="B14">
         <v>61</v>
       </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>3.0800000000000001E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -494,6 +535,12 @@
       <c r="B15">
         <v>71</v>
       </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <v>3.2099999999999997E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -502,101 +549,1635 @@
       <c r="B16">
         <v>81</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>7</v>
+      </c>
+      <c r="E16">
+        <v>3.0700000000000002E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5.5199999999999999E-2</v>
       </c>
       <c r="B17">
         <v>91</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>3.27E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5.6300000000000003E-2</v>
       </c>
       <c r="B18">
         <v>101</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>9</v>
+      </c>
+      <c r="E18">
+        <v>3.39E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5.8500000000000003E-2</v>
       </c>
       <c r="B19">
         <v>111</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="E19">
+        <v>3.3300000000000003E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6.0299999999999999E-2</v>
       </c>
       <c r="B20">
         <v>121</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>11</v>
+      </c>
+      <c r="E20">
+        <v>3.32E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6.1199999999999997E-2</v>
       </c>
       <c r="B21">
         <v>131</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>12</v>
+      </c>
+      <c r="E21">
+        <v>3.3599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>6.25E-2</v>
       </c>
       <c r="B22">
         <v>141</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>13</v>
+      </c>
+      <c r="E22">
+        <v>3.4299999999999997E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="B23">
         <v>151</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>14</v>
+      </c>
+      <c r="E23">
+        <v>3.5799999999999998E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6.5600000000000006E-2</v>
       </c>
       <c r="B24">
         <v>161</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>15</v>
+      </c>
+      <c r="E24">
+        <v>3.6299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="B25">
         <v>171</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>16</v>
+      </c>
+      <c r="E25">
+        <v>3.6400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6.8900000000000003E-2</v>
       </c>
       <c r="B26">
         <v>181</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>17</v>
+      </c>
+      <c r="E26">
+        <v>3.6900000000000002E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>7.0099999999999996E-2</v>
       </c>
       <c r="B27">
         <v>191</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>18</v>
+      </c>
+      <c r="E27">
+        <v>3.6200000000000003E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>7.0800000000000002E-2</v>
       </c>
       <c r="B28">
         <v>201</v>
+      </c>
+      <c r="D28">
+        <v>19</v>
+      </c>
+      <c r="E28">
+        <v>3.6799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>20</v>
+      </c>
+      <c r="E29">
+        <v>3.73E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>21</v>
+      </c>
+      <c r="E30">
+        <v>3.6999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>22</v>
+      </c>
+      <c r="E31">
+        <v>3.7900000000000003E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>23</v>
+      </c>
+      <c r="E32">
+        <v>3.8100000000000002E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>24</v>
+      </c>
+      <c r="E33">
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>25</v>
+      </c>
+      <c r="E34">
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>26</v>
+      </c>
+      <c r="E35">
+        <v>3.8600000000000002E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>27</v>
+      </c>
+      <c r="E36">
+        <v>3.9600000000000003E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>28</v>
+      </c>
+      <c r="E37">
+        <v>3.9600000000000003E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>29</v>
+      </c>
+      <c r="E38">
+        <v>4.0599999999999997E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>30</v>
+      </c>
+      <c r="E39">
+        <v>4.0099999999999997E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>31</v>
+      </c>
+      <c r="E40">
+        <v>4.0899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>32</v>
+      </c>
+      <c r="E41">
+        <v>4.1200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>33</v>
+      </c>
+      <c r="E42">
+        <v>4.1399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>34</v>
+      </c>
+      <c r="E43">
+        <v>4.1799999999999997E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>35</v>
+      </c>
+      <c r="E44">
+        <v>4.2099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>36</v>
+      </c>
+      <c r="E45">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>37</v>
+      </c>
+      <c r="E46">
+        <v>4.2799999999999998E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>38</v>
+      </c>
+      <c r="E47">
+        <v>4.3299999999999998E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <v>39</v>
+      </c>
+      <c r="E48">
+        <v>4.3499999999999997E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>40</v>
+      </c>
+      <c r="E49">
+        <v>4.36E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <v>41</v>
+      </c>
+      <c r="E50">
+        <v>4.3499999999999997E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <v>42</v>
+      </c>
+      <c r="E51">
+        <v>4.3200000000000002E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <v>43</v>
+      </c>
+      <c r="E52">
+        <v>4.41E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <v>44</v>
+      </c>
+      <c r="E53">
+        <v>4.4699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D54">
+        <v>45</v>
+      </c>
+      <c r="E54">
+        <v>4.4900000000000002E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D55">
+        <v>46</v>
+      </c>
+      <c r="E55">
+        <v>4.5499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D56">
+        <v>47</v>
+      </c>
+      <c r="E56">
+        <v>4.5499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <v>48</v>
+      </c>
+      <c r="E57">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <v>49</v>
+      </c>
+      <c r="E58">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D59">
+        <v>50</v>
+      </c>
+      <c r="E59">
+        <v>4.6199999999999998E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D60">
+        <v>51</v>
+      </c>
+      <c r="E60">
+        <v>4.6399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <v>52</v>
+      </c>
+      <c r="E61">
+        <v>4.7100000000000003E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D62">
+        <v>53</v>
+      </c>
+      <c r="E62">
+        <v>4.7100000000000003E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <v>54</v>
+      </c>
+      <c r="E63">
+        <v>4.7399999999999998E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D64">
+        <v>55</v>
+      </c>
+      <c r="E64">
+        <v>4.7100000000000003E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <v>56</v>
+      </c>
+      <c r="E65">
+        <v>4.7500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D66">
+        <v>57</v>
+      </c>
+      <c r="E66">
+        <v>4.7800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D67">
+        <v>58</v>
+      </c>
+      <c r="E67">
+        <v>4.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D68">
+        <v>59</v>
+      </c>
+      <c r="E68">
+        <v>4.87E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D69">
+        <v>60</v>
+      </c>
+      <c r="E69">
+        <v>4.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D70">
+        <v>61</v>
+      </c>
+      <c r="E70">
+        <v>4.9099999999999998E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D71">
+        <v>62</v>
+      </c>
+      <c r="E71">
+        <v>4.9500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D72">
+        <v>63</v>
+      </c>
+      <c r="E72">
+        <v>4.9000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D73">
+        <v>64</v>
+      </c>
+      <c r="E73">
+        <v>4.99E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D74">
+        <v>65</v>
+      </c>
+      <c r="E74">
+        <v>5.0200000000000002E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D75">
+        <v>66</v>
+      </c>
+      <c r="E75">
+        <v>4.9799999999999997E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D76">
+        <v>67</v>
+      </c>
+      <c r="E76">
+        <v>5.0599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D77">
+        <v>68</v>
+      </c>
+      <c r="E77">
+        <v>5.0799999999999998E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D78">
+        <v>69</v>
+      </c>
+      <c r="E78">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D79">
+        <v>70</v>
+      </c>
+      <c r="E79">
+        <v>5.1200000000000002E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D80">
+        <v>71</v>
+      </c>
+      <c r="E80">
+        <v>5.1499999999999997E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D81">
+        <v>72</v>
+      </c>
+      <c r="E81">
+        <v>5.16E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D82">
+        <v>73</v>
+      </c>
+      <c r="E82">
+        <v>5.16E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D83">
+        <v>74</v>
+      </c>
+      <c r="E83">
+        <v>5.1900000000000002E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D84">
+        <v>75</v>
+      </c>
+      <c r="E84">
+        <v>5.2499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D85">
+        <v>76</v>
+      </c>
+      <c r="E85">
+        <v>5.2400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D86">
+        <v>77</v>
+      </c>
+      <c r="E86">
+        <v>5.2400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D87">
+        <v>78</v>
+      </c>
+      <c r="E87">
+        <v>5.3400000000000003E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D88">
+        <v>79</v>
+      </c>
+      <c r="E88">
+        <v>5.2900000000000003E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D89">
+        <v>80</v>
+      </c>
+      <c r="E89">
+        <v>5.3100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D90">
+        <v>81</v>
+      </c>
+      <c r="E90">
+        <v>5.3100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D91">
+        <v>82</v>
+      </c>
+      <c r="E91">
+        <v>5.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D92">
+        <v>83</v>
+      </c>
+      <c r="E92">
+        <v>5.3699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D93">
+        <v>84</v>
+      </c>
+      <c r="E93">
+        <v>5.4100000000000002E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D94">
+        <v>85</v>
+      </c>
+      <c r="E94">
+        <v>5.4100000000000002E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D95">
+        <v>86</v>
+      </c>
+      <c r="E95">
+        <v>5.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D96">
+        <v>87</v>
+      </c>
+      <c r="E96">
+        <v>5.4699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D97">
+        <v>88</v>
+      </c>
+      <c r="E97">
+        <v>5.4300000000000001E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D98">
+        <v>89</v>
+      </c>
+      <c r="E98">
+        <v>5.4800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D99">
+        <v>90</v>
+      </c>
+      <c r="E99">
+        <v>5.4699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D100">
+        <v>91</v>
+      </c>
+      <c r="E100">
+        <v>5.5199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D101">
+        <v>92</v>
+      </c>
+      <c r="E101">
+        <v>5.4800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D102">
+        <v>93</v>
+      </c>
+      <c r="E102">
+        <v>5.5100000000000003E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D103">
+        <v>94</v>
+      </c>
+      <c r="E103">
+        <v>5.45E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D104">
+        <v>95</v>
+      </c>
+      <c r="E104">
+        <v>5.4800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D105">
+        <v>96</v>
+      </c>
+      <c r="E105">
+        <v>5.5100000000000003E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D106">
+        <v>97</v>
+      </c>
+      <c r="E106">
+        <v>5.5399999999999998E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D107">
+        <v>98</v>
+      </c>
+      <c r="E107">
+        <v>5.5500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D108">
+        <v>99</v>
+      </c>
+      <c r="E108">
+        <v>5.57E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D109">
+        <v>100</v>
+      </c>
+      <c r="E109">
+        <v>5.5899999999999998E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D110">
+        <v>101</v>
+      </c>
+      <c r="E110">
+        <v>5.6300000000000003E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D111">
+        <v>102</v>
+      </c>
+      <c r="E111">
+        <v>5.6500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D112">
+        <v>103</v>
+      </c>
+      <c r="E112">
+        <v>5.67E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D113">
+        <v>104</v>
+      </c>
+      <c r="E113">
+        <v>5.6800000000000003E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D114">
+        <v>105</v>
+      </c>
+      <c r="E114">
+        <v>5.7099999999999998E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D115">
+        <v>106</v>
+      </c>
+      <c r="E115">
+        <v>5.7099999999999998E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D116">
+        <v>107</v>
+      </c>
+      <c r="E116">
+        <v>5.74E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D117">
+        <v>108</v>
+      </c>
+      <c r="E117">
+        <v>5.7599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D118">
+        <v>109</v>
+      </c>
+      <c r="E118">
+        <v>5.8000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D119">
+        <v>110</v>
+      </c>
+      <c r="E119">
+        <v>5.8099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D120">
+        <v>111</v>
+      </c>
+      <c r="E120">
+        <v>5.8500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D121">
+        <v>112</v>
+      </c>
+      <c r="E121">
+        <v>5.8500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D122">
+        <v>113</v>
+      </c>
+      <c r="E122">
+        <v>5.8700000000000002E-2</v>
+      </c>
+    </row>
+    <row r="123" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D123">
+        <v>114</v>
+      </c>
+      <c r="E123">
+        <v>5.8999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D124">
+        <v>115</v>
+      </c>
+      <c r="E124">
+        <v>5.9299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D125">
+        <v>116</v>
+      </c>
+      <c r="E125">
+        <v>5.8700000000000002E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D126">
+        <v>117</v>
+      </c>
+      <c r="E126">
+        <v>5.8900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D127">
+        <v>118</v>
+      </c>
+      <c r="E127">
+        <v>5.9299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D128">
+        <v>119</v>
+      </c>
+      <c r="E128">
+        <v>5.9700000000000003E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D129">
+        <v>120</v>
+      </c>
+      <c r="E129">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="130" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D130">
+        <v>121</v>
+      </c>
+      <c r="E130">
+        <v>6.0299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="131" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D131">
+        <v>122</v>
+      </c>
+      <c r="E131">
+        <v>5.9900000000000002E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D132">
+        <v>123</v>
+      </c>
+      <c r="E132">
+        <v>6.0299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D133">
+        <v>124</v>
+      </c>
+      <c r="E133">
+        <v>6.0400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="134" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D134">
+        <v>125</v>
+      </c>
+      <c r="E134">
+        <v>6.0699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="135" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D135">
+        <v>126</v>
+      </c>
+      <c r="E135">
+        <v>6.0600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="136" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D136">
+        <v>127</v>
+      </c>
+      <c r="E136">
+        <v>6.08E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D137">
+        <v>128</v>
+      </c>
+      <c r="E137">
+        <v>6.1199999999999997E-2</v>
+      </c>
+    </row>
+    <row r="138" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D138">
+        <v>129</v>
+      </c>
+      <c r="E138">
+        <v>6.1199999999999997E-2</v>
+      </c>
+    </row>
+    <row r="139" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D139">
+        <v>130</v>
+      </c>
+      <c r="E139">
+        <v>6.1100000000000002E-2</v>
+      </c>
+    </row>
+    <row r="140" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D140">
+        <v>131</v>
+      </c>
+      <c r="E140">
+        <v>6.1199999999999997E-2</v>
+      </c>
+    </row>
+    <row r="141" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D141">
+        <v>132</v>
+      </c>
+      <c r="E141">
+        <v>6.1499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="142" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D142">
+        <v>133</v>
+      </c>
+      <c r="E142">
+        <v>6.1400000000000003E-2</v>
+      </c>
+    </row>
+    <row r="143" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D143">
+        <v>134</v>
+      </c>
+      <c r="E143">
+        <v>6.1800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="144" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D144">
+        <v>135</v>
+      </c>
+      <c r="E144">
+        <v>6.2E-2</v>
+      </c>
+    </row>
+    <row r="145" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D145">
+        <v>136</v>
+      </c>
+      <c r="E145">
+        <v>6.2100000000000002E-2</v>
+      </c>
+    </row>
+    <row r="146" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D146">
+        <v>137</v>
+      </c>
+      <c r="E146">
+        <v>6.2100000000000002E-2</v>
+      </c>
+    </row>
+    <row r="147" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D147">
+        <v>138</v>
+      </c>
+      <c r="E147">
+        <v>6.1800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="148" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D148">
+        <v>139</v>
+      </c>
+      <c r="E148">
+        <v>6.1800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="149" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D149">
+        <v>140</v>
+      </c>
+      <c r="E149">
+        <v>6.2399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="150" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D150">
+        <v>141</v>
+      </c>
+      <c r="E150">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="151" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D151">
+        <v>142</v>
+      </c>
+      <c r="E151">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="152" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D152">
+        <v>143</v>
+      </c>
+      <c r="E152">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="153" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D153">
+        <v>144</v>
+      </c>
+      <c r="E153">
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="154" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D154">
+        <v>145</v>
+      </c>
+      <c r="E154">
+        <v>6.3200000000000006E-2</v>
+      </c>
+    </row>
+    <row r="155" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D155">
+        <v>146</v>
+      </c>
+      <c r="E155">
+        <v>6.3500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="156" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D156">
+        <v>147</v>
+      </c>
+      <c r="E156">
+        <v>6.3399999999999998E-2</v>
+      </c>
+    </row>
+    <row r="157" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D157">
+        <v>148</v>
+      </c>
+      <c r="E157">
+        <v>6.3399999999999998E-2</v>
+      </c>
+    </row>
+    <row r="158" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D158">
+        <v>149</v>
+      </c>
+      <c r="E158">
+        <v>6.3600000000000004E-2</v>
+      </c>
+    </row>
+    <row r="159" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D159">
+        <v>150</v>
+      </c>
+      <c r="E159">
+        <v>6.3700000000000007E-2</v>
+      </c>
+    </row>
+    <row r="160" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D160">
+        <v>151</v>
+      </c>
+      <c r="E160">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="161" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D161">
+        <v>152</v>
+      </c>
+      <c r="E161">
+        <v>6.4299999999999996E-2</v>
+      </c>
+    </row>
+    <row r="162" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D162">
+        <v>153</v>
+      </c>
+      <c r="E162">
+        <v>6.4399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="163" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D163">
+        <v>154</v>
+      </c>
+      <c r="E163">
+        <v>6.4500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="164" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D164">
+        <v>155</v>
+      </c>
+      <c r="E164">
+        <v>6.4799999999999996E-2</v>
+      </c>
+    </row>
+    <row r="165" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D165">
+        <v>156</v>
+      </c>
+      <c r="E165">
+        <v>6.5199999999999994E-2</v>
+      </c>
+    </row>
+    <row r="166" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D166">
+        <v>157</v>
+      </c>
+      <c r="E166">
+        <v>6.5699999999999995E-2</v>
+      </c>
+    </row>
+    <row r="167" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D167">
+        <v>158</v>
+      </c>
+      <c r="E167">
+        <v>6.5600000000000006E-2</v>
+      </c>
+    </row>
+    <row r="168" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D168">
+        <v>159</v>
+      </c>
+      <c r="E168">
+        <v>6.5600000000000006E-2</v>
+      </c>
+    </row>
+    <row r="169" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D169">
+        <v>160</v>
+      </c>
+      <c r="E169">
+        <v>6.54E-2</v>
+      </c>
+    </row>
+    <row r="170" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D170">
+        <v>161</v>
+      </c>
+      <c r="E170">
+        <v>6.5600000000000006E-2</v>
+      </c>
+    </row>
+    <row r="171" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D171">
+        <v>162</v>
+      </c>
+      <c r="E171">
+        <v>6.5699999999999995E-2</v>
+      </c>
+    </row>
+    <row r="172" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D172">
+        <v>163</v>
+      </c>
+      <c r="E172">
+        <v>6.5699999999999995E-2</v>
+      </c>
+    </row>
+    <row r="173" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D173">
+        <v>164</v>
+      </c>
+      <c r="E173">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="174" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D174">
+        <v>165</v>
+      </c>
+      <c r="E174">
+        <v>6.6400000000000001E-2</v>
+      </c>
+    </row>
+    <row r="175" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D175">
+        <v>166</v>
+      </c>
+      <c r="E175">
+        <v>6.6400000000000001E-2</v>
+      </c>
+    </row>
+    <row r="176" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D176">
+        <v>167</v>
+      </c>
+      <c r="E176">
+        <v>6.6600000000000006E-2</v>
+      </c>
+    </row>
+    <row r="177" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D177">
+        <v>168</v>
+      </c>
+      <c r="E177">
+        <v>6.6500000000000004E-2</v>
+      </c>
+    </row>
+    <row r="178" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D178">
+        <v>169</v>
+      </c>
+      <c r="E178">
+        <v>6.6900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="179" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D179">
+        <v>170</v>
+      </c>
+      <c r="E179">
+        <v>6.6799999999999998E-2</v>
+      </c>
+    </row>
+    <row r="180" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D180">
+        <v>171</v>
+      </c>
+      <c r="E180">
+        <v>6.7000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="181" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D181">
+        <v>172</v>
+      </c>
+      <c r="E181">
+        <v>6.7100000000000007E-2</v>
+      </c>
+    </row>
+    <row r="182" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D182">
+        <v>173</v>
+      </c>
+      <c r="E182">
+        <v>6.7799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="183" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D183">
+        <v>174</v>
+      </c>
+      <c r="E183">
+        <v>6.8000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="184" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D184">
+        <v>175</v>
+      </c>
+      <c r="E184">
+        <v>6.83E-2</v>
+      </c>
+    </row>
+    <row r="185" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D185">
+        <v>176</v>
+      </c>
+      <c r="E185">
+        <v>6.8000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="186" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D186">
+        <v>177</v>
+      </c>
+      <c r="E186">
+        <v>6.8000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="187" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D187">
+        <v>178</v>
+      </c>
+      <c r="E187">
+        <v>6.8199999999999997E-2</v>
+      </c>
+    </row>
+    <row r="188" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D188">
+        <v>179</v>
+      </c>
+      <c r="E188">
+        <v>6.8400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="189" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D189">
+        <v>180</v>
+      </c>
+      <c r="E189">
+        <v>6.8599999999999994E-2</v>
+      </c>
+    </row>
+    <row r="190" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D190">
+        <v>181</v>
+      </c>
+      <c r="E190">
+        <v>6.8900000000000003E-2</v>
+      </c>
+    </row>
+    <row r="191" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D191">
+        <v>182</v>
+      </c>
+      <c r="E191">
+        <v>6.88E-2</v>
+      </c>
+    </row>
+    <row r="192" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D192">
+        <v>183</v>
+      </c>
+      <c r="E192">
+        <v>6.9099999999999995E-2</v>
+      </c>
+    </row>
+    <row r="193" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D193">
+        <v>184</v>
+      </c>
+      <c r="E193">
+        <v>6.9000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="194" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D194">
+        <v>185</v>
+      </c>
+      <c r="E194">
+        <v>6.9599999999999995E-2</v>
+      </c>
+    </row>
+    <row r="195" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D195">
+        <v>186</v>
+      </c>
+      <c r="E195">
+        <v>6.9699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="196" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D196">
+        <v>187</v>
+      </c>
+      <c r="E196">
+        <v>6.9900000000000004E-2</v>
+      </c>
+    </row>
+    <row r="197" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D197">
+        <v>188</v>
+      </c>
+      <c r="E197">
+        <v>7.0099999999999996E-2</v>
+      </c>
+    </row>
+    <row r="198" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D198">
+        <v>189</v>
+      </c>
+      <c r="E198">
+        <v>7.0300000000000001E-2</v>
+      </c>
+    </row>
+    <row r="199" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D199">
+        <v>190</v>
+      </c>
+      <c r="E199">
+        <v>7.0199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="200" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D200">
+        <v>191</v>
+      </c>
+      <c r="E200">
+        <v>7.0099999999999996E-2</v>
+      </c>
+    </row>
+    <row r="201" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D201">
+        <v>192</v>
+      </c>
+      <c r="E201">
+        <v>7.0400000000000004E-2</v>
+      </c>
+    </row>
+    <row r="202" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D202">
+        <v>193</v>
+      </c>
+      <c r="E202">
+        <v>7.0199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="203" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D203">
+        <v>194</v>
+      </c>
+      <c r="E203">
+        <v>7.0400000000000004E-2</v>
+      </c>
+    </row>
+    <row r="204" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D204">
+        <v>195</v>
+      </c>
+      <c r="E204">
+        <v>7.0599999999999996E-2</v>
+      </c>
+    </row>
+    <row r="205" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D205">
+        <v>196</v>
+      </c>
+      <c r="E205">
+        <v>7.0900000000000005E-2</v>
+      </c>
+    </row>
+    <row r="206" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D206">
+        <v>197</v>
+      </c>
+      <c r="E206">
+        <v>7.1099999999999997E-2</v>
+      </c>
+    </row>
+    <row r="207" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D207">
+        <v>198</v>
+      </c>
+      <c r="E207">
+        <v>7.0800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="208" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D208">
+        <v>199</v>
+      </c>
+      <c r="E208">
+        <v>7.0900000000000005E-2</v>
+      </c>
+    </row>
+    <row r="209" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D209">
+        <v>200</v>
+      </c>
+      <c r="E209">
+        <v>7.0999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="210" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D210">
+        <v>201</v>
+      </c>
+      <c r="E210">
+        <v>7.0800000000000002E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>